<commit_message>
Update to genomic context graphs
</commit_message>
<xml_diff>
--- a/08_other_files/info_amps.xlsx
+++ b/08_other_files/info_amps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luigui/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luigui/Documents/amps_microbiome/08_other_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81586A6-B3AF-B84D-AAF3-D3FE4C894BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E5D39B-C370-5148-AAD5-5675FCC59367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5420" yWindow="-21600" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{EF9C5A83-DF09-3B48-B88B-3BB3532AE977}"/>
+    <workbookView xWindow="3600" yWindow="500" windowWidth="21600" windowHeight="17500" activeTab="1" xr2:uid="{EF9C5A83-DF09-3B48-B88B-3BB3532AE977}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -896,7 +896,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -924,12 +924,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2026,11 +2021,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{561DEFF6-B190-DE48-8FA8-B76DDB58A61A}">
   <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView zoomScale="188" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="K4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="188" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L21" sqref="L21"/>
+      <selection pane="bottomRight" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5027,8 +5022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B58EF62E-4579-3140-A8F9-0C08C8AF2909}">
   <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="257" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView zoomScale="257" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5215,44 +5210,44 @@
       <c r="A4" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="28">
+      <c r="C4">
         <v>25</v>
       </c>
-      <c r="D4" s="29">
+      <c r="D4" s="5">
         <v>183</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="F4" s="28">
+      <c r="F4">
         <f>IF(D4&lt;21, 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G4" s="28">
-        <v>1</v>
-      </c>
-      <c r="H4" s="27">
-        <v>1</v>
-      </c>
-      <c r="I4" s="28">
-        <v>0</v>
-      </c>
-      <c r="J4" s="27">
-        <v>1</v>
-      </c>
-      <c r="K4" s="28">
-        <v>1</v>
-      </c>
-      <c r="L4" s="27">
-        <v>1</v>
-      </c>
-      <c r="M4" s="31">
-        <v>0</v>
-      </c>
-      <c r="N4" s="28">
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1</v>
+      </c>
+      <c r="M4" s="24">
+        <v>0</v>
+      </c>
+      <c r="N4">
         <f>SUM(F4:M4)</f>
         <v>5</v>
       </c>
@@ -5317,44 +5312,44 @@
       <c r="A8" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="28">
+      <c r="C8">
         <v>26</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="5">
         <v>69</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="F8" s="28">
+      <c r="F8">
         <f>IF(D8&lt;21, 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="G8" s="28">
-        <v>1</v>
-      </c>
-      <c r="H8" s="27">
-        <v>1</v>
-      </c>
-      <c r="I8" s="28">
-        <v>0</v>
-      </c>
-      <c r="J8" s="27">
-        <v>1</v>
-      </c>
-      <c r="K8" s="28">
-        <v>1</v>
-      </c>
-      <c r="L8" s="27">
-        <v>1</v>
-      </c>
-      <c r="M8" s="31">
-        <v>0</v>
-      </c>
-      <c r="N8" s="28">
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8" s="1">
+        <v>1</v>
+      </c>
+      <c r="M8" s="24">
+        <v>0</v>
+      </c>
+      <c r="N8">
         <f>SUM(F8:M8)</f>
         <v>5</v>
       </c>
@@ -5442,44 +5437,44 @@
       <c r="A10" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="28">
+      <c r="C10">
         <v>41</v>
       </c>
-      <c r="D10" s="32">
-        <v>1</v>
-      </c>
-      <c r="E10" s="30" t="s">
+      <c r="D10" s="27">
+        <v>1</v>
+      </c>
+      <c r="E10" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10">
         <f>IF(D10&lt;21, 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="G10" s="28">
-        <v>1</v>
-      </c>
-      <c r="H10" s="27">
-        <v>1</v>
-      </c>
-      <c r="I10" s="28">
-        <v>0</v>
-      </c>
-      <c r="J10" s="27">
-        <v>1</v>
-      </c>
-      <c r="K10" s="28">
-        <v>1</v>
-      </c>
-      <c r="L10" s="27">
-        <v>1</v>
-      </c>
-      <c r="M10" s="31">
-        <v>0</v>
-      </c>
-      <c r="N10" s="28">
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10" s="1">
+        <v>1</v>
+      </c>
+      <c r="M10" s="24">
+        <v>0</v>
+      </c>
+      <c r="N10">
         <f>SUM(F10:M10)</f>
         <v>6</v>
       </c>
@@ -5500,44 +5495,44 @@
       <c r="A11" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C11" s="28">
+      <c r="C11">
         <v>13</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D11" s="27">
         <v>7</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11">
         <f>IF(D11&lt;21, 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="G11" s="27">
+      <c r="G11" s="1">
         <v>2</v>
       </c>
-      <c r="H11" s="27">
-        <v>1</v>
-      </c>
-      <c r="I11" s="28">
-        <v>0</v>
-      </c>
-      <c r="J11" s="27">
-        <v>1</v>
-      </c>
-      <c r="K11" s="28">
-        <v>1</v>
-      </c>
-      <c r="L11" s="31">
-        <v>0</v>
-      </c>
-      <c r="M11" s="31">
-        <v>0</v>
-      </c>
-      <c r="N11" s="28">
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11" s="24">
+        <v>0</v>
+      </c>
+      <c r="M11" s="24">
+        <v>0</v>
+      </c>
+      <c r="N11">
         <f>SUM(F11:M11)</f>
         <v>6</v>
       </c>

</xml_diff>